<commit_message>
added new AOD resources
</commit_message>
<xml_diff>
--- a/Module Code Generator.xlsx
+++ b/Module Code Generator.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intra\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intra\OneDrive\Desktop\Rolodex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8520F820-00A2-46F4-8D99-EEB31D370A92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E41F451-6044-40E2-AEBE-E4877D23479E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="13770" xr2:uid="{A9122E04-BE42-49C0-8E95-A2ED7E8620F5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Accordion Title</t>
   </si>
@@ -68,25 +68,52 @@
     <t>ENTER INTO UI</t>
   </si>
   <si>
-    <t>HL_FindAHelpline</t>
-  </si>
-  <si>
-    <t>Find a Helpline</t>
-  </si>
-  <si>
-    <t>Hldata</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
-    <t>mod_Accordion_ui('HL_FindAHelpline')</t>
-  </si>
-  <si>
-    <t>mod_Accordion_server('HL_FindAHelpline', selector=selection, data=Hldata, title = c('Find a Helpline'), Visible = T)</t>
-  </si>
-  <si>
-    <t>mod_info_server('HL_FindAHelpline', selector = selection, data = Hldata, rownametitle = c('Find a Helpline'), phone = F, website = T)</t>
+    <t>AA Meetings</t>
+  </si>
+  <si>
+    <t>AODdata</t>
+  </si>
+  <si>
+    <t>mod_Accordion_ui('AOD_NaloxoneCal')</t>
+  </si>
+  <si>
+    <t>mod_Accordion_server('AOD_NaloxoneCal', selector=selection, data=AODdata, title = c('OASAS Naloxone Training Calendar'), Visible = T)</t>
+  </si>
+  <si>
+    <t>mod_info_server('AOD_NaloxoneCal', selector = selection, data = AODdata, rownametitle = c('OASAS Naloxone Training Calendar'), phone = F, website = T)</t>
+  </si>
+  <si>
+    <t>mod_Accordion_ui('AOD_SMART')</t>
+  </si>
+  <si>
+    <t>mod_Accordion_server('AOD_SMART', selector=selection, data=AODdata, title = c('SMART Recovery Meetings'), Visible = T)</t>
+  </si>
+  <si>
+    <t>mod_info_server('AOD_SMART', selector = selection, data = AODdata, rownametitle = c('SMART Recovery Meetings'), phone = F, website = T)</t>
+  </si>
+  <si>
+    <t>mod_Accordion_ui('AOD_Refuge')</t>
+  </si>
+  <si>
+    <t>mod_Accordion_server('AOD_Refuge', selector=selection, data=AODdata, title = c('Refuge Recovery Meetings'), Visible = T)</t>
+  </si>
+  <si>
+    <t>mod_info_server('AOD_Refuge', selector = selection, data = AODdata, rownametitle = c('Refuge Recovery Meetings'), phone = F, website = T)</t>
+  </si>
+  <si>
+    <t>AOD_Aameetings</t>
+  </si>
+  <si>
+    <t>mod_Accordion_ui('AOD_Aameetings')</t>
+  </si>
+  <si>
+    <t>mod_Accordion_server('AOD_Aameetings', selector=selection, data=AODdata, title = c('AA Meetings'), Visible = T)</t>
+  </si>
+  <si>
+    <t>mod_info_server('AOD_Aameetings', selector = selection, data = AODdata, rownametitle = c('AA Meetings'), phone = F, website = T)</t>
   </si>
 </sst>
 </file>
@@ -480,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EBEBDEC-DB4C-4547-B739-F553404489A4}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -519,19 +546,19 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>3</v>
@@ -543,7 +570,7 @@
       </c>
       <c r="B4" s="3" t="str">
         <f>"mod_Accordion_ui("&amp;"'"&amp;A2&amp;"'"&amp;")"</f>
-        <v>mod_Accordion_ui('HL_FindAHelpline')</v>
+        <v>mod_Accordion_ui('AOD_Aameetings')</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -552,7 +579,7 @@
       </c>
       <c r="B5" s="3" t="str">
         <f>"mod_Accordion_server("&amp;"'"&amp;A2&amp;"', selector=selection, data="&amp;C2&amp;", title = c('"&amp;D2&amp;"'), Visible = T)"</f>
-        <v>mod_Accordion_server('HL_FindAHelpline', selector=selection, data=Hldata, title = c('Find a Helpline'), Visible = T)</v>
+        <v>mod_Accordion_server('AOD_Aameetings', selector=selection, data=AODdata, title = c('AA Meetings'), Visible = T)</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -561,7 +588,7 @@
       </c>
       <c r="B6" s="3" t="str">
         <f>"mod_info_server('"&amp;A2&amp;"', selector = selection, data = "&amp;C2&amp;", rownametitle = c('"&amp;B2&amp;"'), phone = "&amp;E2&amp;", website = "&amp;F2&amp;")"</f>
-        <v>mod_info_server('HL_FindAHelpline', selector = selection, data = Hldata, rownametitle = c('Find a Helpline'), phone = F, website = T)</v>
+        <v>mod_info_server('AOD_Aameetings', selector = selection, data = AODdata, rownametitle = c('AA Meetings'), phone = F, website = T)</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -573,9 +600,7 @@
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="6"/>
       <c r="D11" s="7"/>
@@ -584,17 +609,12 @@
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A12" s="1"/>
       <c r="D12" s="6"/>
       <c r="E12" s="8"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="E13" s="1"/>
@@ -611,23 +631,71 @@
       <c r="C16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C22" s="4"/>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C18" s="4"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added NUA Spanish line
</commit_message>
<xml_diff>
--- a/Module Code Generator.xlsx
+++ b/Module Code Generator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intra\OneDrive\Desktop\Rolodex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E41F451-6044-40E2-AEBE-E4877D23479E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DC6451-BCD4-46AE-BF92-9AB25A5D6F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="13770" xr2:uid="{A9122E04-BE42-49C0-8E95-A2ED7E8620F5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{A9122E04-BE42-49C0-8E95-A2ED7E8620F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Accordion Title</t>
   </si>
@@ -68,52 +68,37 @@
     <t>ENTER INTO UI</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>AA Meetings</t>
-  </si>
-  <si>
     <t>AODdata</t>
   </si>
   <si>
-    <t>mod_Accordion_ui('AOD_NaloxoneCal')</t>
-  </si>
-  <si>
-    <t>mod_Accordion_server('AOD_NaloxoneCal', selector=selection, data=AODdata, title = c('OASAS Naloxone Training Calendar'), Visible = T)</t>
-  </si>
-  <si>
-    <t>mod_info_server('AOD_NaloxoneCal', selector = selection, data = AODdata, rownametitle = c('OASAS Naloxone Training Calendar'), phone = F, website = T)</t>
-  </si>
-  <si>
-    <t>mod_Accordion_ui('AOD_SMART')</t>
-  </si>
-  <si>
-    <t>mod_Accordion_server('AOD_SMART', selector=selection, data=AODdata, title = c('SMART Recovery Meetings'), Visible = T)</t>
-  </si>
-  <si>
-    <t>mod_info_server('AOD_SMART', selector = selection, data = AODdata, rownametitle = c('SMART Recovery Meetings'), phone = F, website = T)</t>
-  </si>
-  <si>
-    <t>mod_Accordion_ui('AOD_Refuge')</t>
-  </si>
-  <si>
-    <t>mod_Accordion_server('AOD_Refuge', selector=selection, data=AODdata, title = c('Refuge Recovery Meetings'), Visible = T)</t>
-  </si>
-  <si>
-    <t>mod_info_server('AOD_Refuge', selector = selection, data = AODdata, rownametitle = c('Refuge Recovery Meetings'), phone = F, website = T)</t>
-  </si>
-  <si>
-    <t>AOD_Aameetings</t>
-  </si>
-  <si>
-    <t>mod_Accordion_ui('AOD_Aameetings')</t>
-  </si>
-  <si>
-    <t>mod_Accordion_server('AOD_Aameetings', selector=selection, data=AODdata, title = c('AA Meetings'), Visible = T)</t>
-  </si>
-  <si>
-    <t>mod_info_server('AOD_Aameetings', selector = selection, data = AODdata, rownametitle = c('AA Meetings'), phone = F, website = T)</t>
+    <t>tel:18009285330</t>
+  </si>
+  <si>
+    <t>https://neverusealone.com/</t>
+  </si>
+  <si>
+    <t>AOD</t>
+  </si>
+  <si>
+    <t>Off</t>
+  </si>
+  <si>
+    <t>National anonymous hotline - Will stay on the phone with you if you use alone and will call for help to your address if you experience an overdose - Overdose prevention</t>
+  </si>
+  <si>
+    <t>AOD_NUAspanish</t>
+  </si>
+  <si>
+    <t>Never Use Alone (Spanish)</t>
+  </si>
+  <si>
+    <t>mod_Accordion_ui('AOD_NUAspanish')</t>
+  </si>
+  <si>
+    <t>mod_Accordion_server('AOD_NUAspanish', selector=selection, data=AODdata, title = c('Never Use Alone (Spanish)'), Visible = T)</t>
+  </si>
+  <si>
+    <t>mod_info_server('AOD_NUAspanish', selector = selection, data = AODdata, rownametitle = c('Never Use Alone (Spanish)'), phone = T, website = T)</t>
   </si>
 </sst>
 </file>
@@ -178,7 +163,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -192,6 +177,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -507,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EBEBDEC-DB4C-4547-B739-F553404489A4}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -524,7 +510,7 @@
     <col min="8" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -544,54 +530,54 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>11</v>
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="3" t="str">
         <f>"mod_Accordion_ui("&amp;"'"&amp;A2&amp;"'"&amp;")"</f>
-        <v>mod_Accordion_ui('AOD_Aameetings')</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+        <v>mod_Accordion_ui('AOD_NUAspanish')</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="3" t="str">
         <f>"mod_Accordion_server("&amp;"'"&amp;A2&amp;"', selector=selection, data="&amp;C2&amp;", title = c('"&amp;D2&amp;"'), Visible = T)"</f>
-        <v>mod_Accordion_server('AOD_Aameetings', selector=selection, data=AODdata, title = c('AA Meetings'), Visible = T)</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+        <v>mod_Accordion_server('AOD_NUAspanish', selector=selection, data=AODdata, title = c('Never Use Alone (Spanish)'), Visible = T)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="3" t="str">
         <f>"mod_info_server('"&amp;A2&amp;"', selector = selection, data = "&amp;C2&amp;", rownametitle = c('"&amp;B2&amp;"'), phone = "&amp;E2&amp;", website = "&amp;F2&amp;")"</f>
-        <v>mod_info_server('AOD_Aameetings', selector = selection, data = AODdata, rownametitle = c('AA Meetings'), phone = F, website = T)</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+        <v>mod_info_server('AOD_NUAspanish', selector = selection, data = AODdata, rownametitle = c('Never Use Alone (Spanish)'), phone = T, website = T)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="5"/>
       <c r="D10" s="1"/>
@@ -599,7 +585,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="6"/>
@@ -608,97 +594,67 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="D12" s="6"/>
       <c r="E12" s="8"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="C16" s="1"/>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="C18" s="4"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C13" r:id="rId1" xr:uid="{D99E8F92-F49B-4427-8EBD-4B132661AD4D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added campusdrugprevention.gov drug index.
</commit_message>
<xml_diff>
--- a/Module Code Generator.xlsx
+++ b/Module Code Generator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intra\OneDrive\Desktop\Rolodex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F6409AB-14C4-4BA6-A0B2-83A28F0749E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A27F3B3B-28B0-4E09-8D00-80CE0D50A566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{A9122E04-BE42-49C0-8E95-A2ED7E8620F5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Accordion Title</t>
   </si>
@@ -74,21 +74,9 @@
     <t>Off</t>
   </si>
   <si>
-    <t>The Brave App</t>
-  </si>
-  <si>
-    <t>https://www.brave.coop/overdose-detection-app</t>
-  </si>
-  <si>
-    <t>Set up a Rescue Plan that details how, when, and who will be sent for help in the event you overdose. Anonymously and privately connect to a Brave Supporter through the app before you use drugs alone. They will stay on the line with you until you feel that you are safe.</t>
-  </si>
-  <si>
     <t>AODdata()</t>
   </si>
   <si>
-    <t>AOD_BraveAPP</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
@@ -99,6 +87,24 @@
   </si>
   <si>
     <t>mod_info_server('AOD_BraveAPP', selector = selection, data = AODdata(), rownametitle = c('The Brave App'), phone = F, website = T)</t>
+  </si>
+  <si>
+    <t>Drug Index (CampusDrugPrevention.gov)</t>
+  </si>
+  <si>
+    <t>https://www.campusdrugprevention.gov/drugs</t>
+  </si>
+  <si>
+    <t>The CampusDrugPrevention.gov Drug Index is a one-stop reference for everything related to drugs -- from their appearance, paraphernalia, effects on the body, and more.</t>
+  </si>
+  <si>
+    <t>AOD_CampusDrugPrevINDEX</t>
+  </si>
+  <si>
+    <t>mod_Accordion_server('AOD_CampusDrugPrevINDEX', selector=selection, data=AODdata(), title = c('Drug Index (CampusDrugPrevention.gov)'), Visible = T)</t>
+  </si>
+  <si>
+    <t>mod_info_server('AOD_CampusDrugPrevINDEX', selector = selection, data = AODdata(), rownametitle = c('Drug Index (CampusDrugPrevention.gov)'), phone = F, website = T)</t>
   </si>
 </sst>
 </file>
@@ -143,6 +149,7 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -168,7 +175,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -183,7 +190,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -502,7 +513,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B9" sqref="B9:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -538,19 +549,19 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>3</v>
@@ -562,7 +573,7 @@
       </c>
       <c r="B4" s="3" t="str">
         <f>"mod_Accordion_ui("&amp;"'"&amp;A2&amp;"'"&amp;")"</f>
-        <v>mod_Accordion_ui('AOD_BraveAPP')</v>
+        <v>mod_Accordion_ui('AOD_CampusDrugPrevINDEX')</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -571,7 +582,7 @@
       </c>
       <c r="B5" s="3" t="str">
         <f>"mod_Accordion_server("&amp;"'"&amp;A2&amp;"', selector=selection, data="&amp;C2&amp;", title = c('"&amp;D2&amp;"'), Visible = T)"</f>
-        <v>mod_Accordion_server('AOD_BraveAPP', selector=selection, data=AODdata(), title = c('The Brave App'), Visible = T)</v>
+        <v>mod_Accordion_server('AOD_CampusDrugPrevINDEX', selector=selection, data=AODdata(), title = c('Drug Index (CampusDrugPrevention.gov)'), Visible = T)</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -580,12 +591,19 @@
       </c>
       <c r="B6" s="3" t="str">
         <f>"mod_info_server('"&amp;A2&amp;"', selector = selection, data = "&amp;C2&amp;", rownametitle = c('"&amp;B2&amp;"'), phone = "&amp;E2&amp;", website = "&amp;F2&amp;")"</f>
-        <v>mod_info_server('AOD_BraveAPP', selector = selection, data = AODdata(), rownametitle = c('The Brave App'), phone = F, website = T)</v>
+        <v>mod_info_server('AOD_CampusDrugPrevINDEX', selector = selection, data = AODdata(), rownametitle = c('Drug Index (CampusDrugPrevention.gov)'), phone = F, website = T)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B9" s="11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
-      <c r="B10" s="5"/>
+      <c r="B10" s="12" t="s">
+        <v>22</v>
+      </c>
       <c r="D10" s="1"/>
       <c r="E10" s="5"/>
       <c r="F10" s="1"/>
@@ -608,12 +626,12 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="9"/>
       <c r="D13" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -624,7 +642,7 @@
         <v>11</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -637,20 +655,20 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C16" s="1"/>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C18" s="4"/>
     </row>

</xml_diff>

<commit_message>
NYS Prob Gambling Main Website added
</commit_message>
<xml_diff>
--- a/Module Code Generator.xlsx
+++ b/Module Code Generator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intra\OneDrive\Desktop\Rolodex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3AF5554-2AE4-474D-8CED-D02533DF444E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52ED2383-6CEF-41BF-8145-55D73FD83060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="1500" windowWidth="19200" windowHeight="9970" xr2:uid="{A9122E04-BE42-49C0-8E95-A2ED7E8620F5}"/>
+    <workbookView xWindow="27860" yWindow="8720" windowWidth="19200" windowHeight="9970" xr2:uid="{A9122E04-BE42-49C0-8E95-A2ED7E8620F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Accordion Title</t>
   </si>
@@ -68,40 +68,25 @@
     <t>ENTER INTO UI</t>
   </si>
   <si>
-    <t>SLGBT()</t>
-  </si>
-  <si>
-    <t>The Trevor Project</t>
-  </si>
-  <si>
-    <t>tel:1-866-488-7386</t>
-  </si>
-  <si>
-    <t>https://www.thetrevorproject.org/get-help/</t>
-  </si>
-  <si>
-    <t>24/7, 365 days a year</t>
-  </si>
-  <si>
-    <t>SLGBT</t>
-  </si>
-  <si>
-    <t>Off</t>
-  </si>
-  <si>
-    <t>The Trevor Project is a nonprofit organization that provides crisis intervention and suicide prevention services for youth. They offer guidance and resources to parents and educators to foster safe, accepting, and inclusive environments for all youth, at home, schools, and colleges. Text 678678</t>
-  </si>
-  <si>
-    <t>LGBTQ_TrevorProject</t>
-  </si>
-  <si>
-    <t>mod_Accordion_ui('LGBTQ_TrevorProject')</t>
-  </si>
-  <si>
-    <t>mod_Accordion_server('LGBTQ_TrevorProject', selector=selection, data=SLGBT(), title = c('The Trevor Project'), Visible = T)</t>
-  </si>
-  <si>
-    <t>mod_info_server('LGBTQ_TrevorProject', selector = selection, data = SLGBT(), rownametitle = c('The Trevor Project'), phone = T, website = T)</t>
+    <t>NYS Problem Gambling Help</t>
+  </si>
+  <si>
+    <t>GAMB_NYSmainwebsite</t>
+  </si>
+  <si>
+    <t>GAMBdata()</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>mod_Accordion_ui('GAMB_NYSmainwebsite')</t>
+  </si>
+  <si>
+    <t>mod_Accordion_server('GAMB_NYSmainwebsite', selector=selection, data=GAMBdata(), title = c('NYS Problem Gambling Help'), Visible = T)</t>
+  </si>
+  <si>
+    <t>mod_info_server('GAMB_NYSmainwebsite', selector = selection, data = GAMBdata(), rownametitle = c('NYS Problem Gambling Help'), phone = F, website = T)</t>
   </si>
 </sst>
 </file>
@@ -506,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EBEBDEC-DB4C-4547-B739-F553404489A4}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -543,19 +528,19 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>3</v>
@@ -567,7 +552,7 @@
       </c>
       <c r="B4" s="3" t="str">
         <f>"mod_Accordion_ui("&amp;"'"&amp;A2&amp;"'"&amp;")"</f>
-        <v>mod_Accordion_ui('LGBTQ_TrevorProject')</v>
+        <v>mod_Accordion_ui('GAMB_NYSmainwebsite')</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -576,7 +561,7 @@
       </c>
       <c r="B5" s="3" t="str">
         <f>"mod_Accordion_server("&amp;"'"&amp;A2&amp;"', selector=selection, data="&amp;C2&amp;", title = c('"&amp;D2&amp;"'), Visible = T)"</f>
-        <v>mod_Accordion_server('LGBTQ_TrevorProject', selector=selection, data=SLGBT(), title = c('The Trevor Project'), Visible = T)</v>
+        <v>mod_Accordion_server('GAMB_NYSmainwebsite', selector=selection, data=GAMBdata(), title = c('NYS Problem Gambling Help'), Visible = T)</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -585,7 +570,7 @@
       </c>
       <c r="B6" s="3" t="str">
         <f>"mod_info_server('"&amp;A2&amp;"', selector = selection, data = "&amp;C2&amp;", rownametitle = c('"&amp;B2&amp;"'), phone = "&amp;E2&amp;", website = "&amp;F2&amp;")"</f>
-        <v>mod_info_server('LGBTQ_TrevorProject', selector = selection, data = SLGBT(), rownametitle = c('The Trevor Project'), phone = T, website = T)</v>
+        <v>mod_info_server('GAMB_NYSmainwebsite', selector = selection, data = GAMBdata(), rownametitle = c('NYS Problem Gambling Help'), phone = F, website = T)</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -594,29 +579,15 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
@@ -625,15 +596,15 @@
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="D12" s="5"/>
       <c r="E12" s="7"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="8"/>
       <c r="D13" s="1"/>
@@ -644,16 +615,10 @@
       <c r="I13" s="9"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="C14" s="1"/>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="C15" s="1"/>
       <c r="E15" s="1"/>
     </row>

</xml_diff>

<commit_message>
Added "Know the Odds" Problem Gamb Resource
</commit_message>
<xml_diff>
--- a/Module Code Generator.xlsx
+++ b/Module Code Generator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intra\OneDrive\Desktop\Rolodex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intra\Desktop\Rolodex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52ED2383-6CEF-41BF-8145-55D73FD83060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB11E45C-FB92-4A51-A0E2-D546FE99CCF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27860" yWindow="8720" windowWidth="19200" windowHeight="9970" xr2:uid="{A9122E04-BE42-49C0-8E95-A2ED7E8620F5}"/>
+    <workbookView xWindow="-3005" yWindow="-10890" windowWidth="19380" windowHeight="10260" xr2:uid="{A9122E04-BE42-49C0-8E95-A2ED7E8620F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,25 +68,25 @@
     <t>ENTER INTO UI</t>
   </si>
   <si>
-    <t>NYS Problem Gambling Help</t>
-  </si>
-  <si>
-    <t>GAMB_NYSmainwebsite</t>
-  </si>
-  <si>
     <t>GAMBdata()</t>
   </si>
   <si>
     <t>F</t>
   </si>
   <si>
-    <t>mod_Accordion_ui('GAMB_NYSmainwebsite')</t>
-  </si>
-  <si>
-    <t>mod_Accordion_server('GAMB_NYSmainwebsite', selector=selection, data=GAMBdata(), title = c('NYS Problem Gambling Help'), Visible = T)</t>
-  </si>
-  <si>
-    <t>mod_info_server('GAMB_NYSmainwebsite', selector = selection, data = GAMBdata(), rownametitle = c('NYS Problem Gambling Help'), phone = F, website = T)</t>
+    <t>GAMB_Knowtheodds</t>
+  </si>
+  <si>
+    <t>Know the Odds</t>
+  </si>
+  <si>
+    <t>mod_Accordion_ui('GAMB_Knowtheodds')</t>
+  </si>
+  <si>
+    <t>mod_Accordion_server('GAMB_Knowtheodds', selector=selection, data=GAMBdata(), title = c('Know the Odds'), Visible = T)</t>
+  </si>
+  <si>
+    <t>mod_info_server('GAMB_Knowtheodds', selector = selection, data = GAMBdata(), rownametitle = c('Know the Odds'), phone = F, website = T)</t>
   </si>
 </sst>
 </file>
@@ -491,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EBEBDEC-DB4C-4547-B739-F553404489A4}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -528,19 +528,19 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>3</v>
@@ -552,7 +552,7 @@
       </c>
       <c r="B4" s="3" t="str">
         <f>"mod_Accordion_ui("&amp;"'"&amp;A2&amp;"'"&amp;")"</f>
-        <v>mod_Accordion_ui('GAMB_NYSmainwebsite')</v>
+        <v>mod_Accordion_ui('GAMB_Knowtheodds')</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -561,7 +561,7 @@
       </c>
       <c r="B5" s="3" t="str">
         <f>"mod_Accordion_server("&amp;"'"&amp;A2&amp;"', selector=selection, data="&amp;C2&amp;", title = c('"&amp;D2&amp;"'), Visible = T)"</f>
-        <v>mod_Accordion_server('GAMB_NYSmainwebsite', selector=selection, data=GAMBdata(), title = c('NYS Problem Gambling Help'), Visible = T)</v>
+        <v>mod_Accordion_server('GAMB_Knowtheodds', selector=selection, data=GAMBdata(), title = c('Know the Odds'), Visible = T)</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -570,7 +570,7 @@
       </c>
       <c r="B6" s="3" t="str">
         <f>"mod_info_server('"&amp;A2&amp;"', selector = selection, data = "&amp;C2&amp;", rownametitle = c('"&amp;B2&amp;"'), phone = "&amp;E2&amp;", website = "&amp;F2&amp;")"</f>
-        <v>mod_info_server('GAMB_NYSmainwebsite', selector = selection, data = GAMBdata(), rownametitle = c('NYS Problem Gambling Help'), phone = F, website = T)</v>
+        <v>mod_info_server('GAMB_Knowtheodds', selector = selection, data = GAMBdata(), rownametitle = c('Know the Odds'), phone = F, website = T)</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added Career Services to AcaData()
</commit_message>
<xml_diff>
--- a/Module Code Generator.xlsx
+++ b/Module Code Generator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intra\Desktop\Rolodex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB11E45C-FB92-4A51-A0E2-D546FE99CCF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA89FD8-ADCF-4D7E-BC77-0BBAF65A185B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3005" yWindow="-10890" windowWidth="19380" windowHeight="10260" xr2:uid="{A9122E04-BE42-49C0-8E95-A2ED7E8620F5}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="13770" xr2:uid="{A9122E04-BE42-49C0-8E95-A2ED7E8620F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Accordion Title</t>
   </si>
@@ -68,25 +68,22 @@
     <t>ENTER INTO UI</t>
   </si>
   <si>
-    <t>GAMBdata()</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>GAMB_Knowtheodds</t>
-  </si>
-  <si>
-    <t>Know the Odds</t>
-  </si>
-  <si>
-    <t>mod_Accordion_ui('GAMB_Knowtheodds')</t>
-  </si>
-  <si>
-    <t>mod_Accordion_server('GAMB_Knowtheodds', selector=selection, data=GAMBdata(), title = c('Know the Odds'), Visible = T)</t>
-  </si>
-  <si>
-    <t>mod_info_server('GAMB_Knowtheodds', selector = selection, data = GAMBdata(), rownametitle = c('Know the Odds'), phone = F, website = T)</t>
+    <t>UAlbany Career Services</t>
+  </si>
+  <si>
+    <t>ACA_CareerServices</t>
+  </si>
+  <si>
+    <t>ACAdata()</t>
+  </si>
+  <si>
+    <t>mod_Accordion_ui('ACA_CareerServices')</t>
+  </si>
+  <si>
+    <t>mod_Accordion_server('ACA_CareerServices', selector=selection, data=ACAdata(), title = c('UAlbany Career Services'), Visible = T)</t>
+  </si>
+  <si>
+    <t>mod_info_server('ACA_CareerServices', selector = selection, data = ACAdata(), rownametitle = c('UAlbany Career Services'), phone = T, website = T)</t>
   </si>
 </sst>
 </file>
@@ -492,7 +489,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -528,19 +525,19 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>3</v>
@@ -552,7 +549,7 @@
       </c>
       <c r="B4" s="3" t="str">
         <f>"mod_Accordion_ui("&amp;"'"&amp;A2&amp;"'"&amp;")"</f>
-        <v>mod_Accordion_ui('GAMB_Knowtheodds')</v>
+        <v>mod_Accordion_ui('ACA_CareerServices')</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -561,7 +558,7 @@
       </c>
       <c r="B5" s="3" t="str">
         <f>"mod_Accordion_server("&amp;"'"&amp;A2&amp;"', selector=selection, data="&amp;C2&amp;", title = c('"&amp;D2&amp;"'), Visible = T)"</f>
-        <v>mod_Accordion_server('GAMB_Knowtheodds', selector=selection, data=GAMBdata(), title = c('Know the Odds'), Visible = T)</v>
+        <v>mod_Accordion_server('ACA_CareerServices', selector=selection, data=ACAdata(), title = c('UAlbany Career Services'), Visible = T)</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -570,7 +567,7 @@
       </c>
       <c r="B6" s="3" t="str">
         <f>"mod_info_server('"&amp;A2&amp;"', selector = selection, data = "&amp;C2&amp;", rownametitle = c('"&amp;B2&amp;"'), phone = "&amp;E2&amp;", website = "&amp;F2&amp;")"</f>
-        <v>mod_info_server('GAMB_Knowtheodds', selector = selection, data = GAMBdata(), rownametitle = c('Know the Odds'), phone = F, website = T)</v>
+        <v>mod_info_server('ACA_CareerServices', selector = selection, data = ACAdata(), rownametitle = c('UAlbany Career Services'), phone = T, website = T)</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -579,14 +576,14 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G10" s="1"/>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="5"/>
@@ -597,7 +594,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="7"/>

</xml_diff>

<commit_message>
Added IPV and 3 other resources
</commit_message>
<xml_diff>
--- a/Module Code Generator.xlsx
+++ b/Module Code Generator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intra\Desktop\Rolodex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA89FD8-ADCF-4D7E-BC77-0BBAF65A185B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5C3473-6698-44F3-8BAF-962AB85EEEFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="13770" xr2:uid="{A9122E04-BE42-49C0-8E95-A2ED7E8620F5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{A9122E04-BE42-49C0-8E95-A2ED7E8620F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Accordion Title</t>
   </si>
@@ -68,29 +68,47 @@
     <t>ENTER INTO UI</t>
   </si>
   <si>
-    <t>UAlbany Career Services</t>
-  </si>
-  <si>
-    <t>ACA_CareerServices</t>
-  </si>
-  <si>
-    <t>ACAdata()</t>
-  </si>
-  <si>
-    <t>mod_Accordion_ui('ACA_CareerServices')</t>
-  </si>
-  <si>
-    <t>mod_Accordion_server('ACA_CareerServices', selector=selection, data=ACAdata(), title = c('UAlbany Career Services'), Visible = T)</t>
-  </si>
-  <si>
-    <t>mod_info_server('ACA_CareerServices', selector = selection, data = ACAdata(), rownametitle = c('UAlbany Career Services'), phone = T, website = T)</t>
+    <t>International Student and Scholar Services</t>
+  </si>
+  <si>
+    <t>mod_Accordion_ui('FHF_The Food Pantries Food Connect Map')</t>
+  </si>
+  <si>
+    <t>mod_Accordion_server('FHF_The Food Pantries Food Connect Map', selector=selection, data=FHFdata(), title = c('The Food Pantries Food Connect Map'), Visible = T)</t>
+  </si>
+  <si>
+    <t>mod_info_server('FHF_The Food Pantries Food Connect Map', selector = selection, data = FHFdata(), rownametitle = c('The Food Pantries Food Connect Map'), phone = F, website = T)</t>
+  </si>
+  <si>
+    <t>mod_Accordion_ui('FHF_Capital Roots')</t>
+  </si>
+  <si>
+    <t>mod_Accordion_server('FHF_Capital Roots', selector=selection, data=FHFdata(), title = c('Capital Roots'), Visible = T)</t>
+  </si>
+  <si>
+    <t>mod_info_server('FHF_Capital Roots', selector = selection, data = FHFdata(), rownametitle = c('Capital Roots'), phone = T, website = T)</t>
+  </si>
+  <si>
+    <t>Aca_International Student and Scholar Services</t>
+  </si>
+  <si>
+    <t>Acadata()</t>
+  </si>
+  <si>
+    <t>mod_Accordion_ui('Aca_International Student and Scholar Services')</t>
+  </si>
+  <si>
+    <t>mod_Accordion_server('Aca_International Student and Scholar Services', selector=selection, data=Acadata(), title = c('International Student and Scholar Services'), Visible = T)</t>
+  </si>
+  <si>
+    <t>mod_info_server('Aca_International Student and Scholar Services', selector = selection, data = Acadata(), rownametitle = c('International Student and Scholar Services'), phone = T, website = T)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +150,11 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -154,7 +177,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -171,6 +194,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -486,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EBEBDEC-DB4C-4547-B739-F553404489A4}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -525,15 +552,15 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -549,7 +576,7 @@
       </c>
       <c r="B4" s="3" t="str">
         <f>"mod_Accordion_ui("&amp;"'"&amp;A2&amp;"'"&amp;")"</f>
-        <v>mod_Accordion_ui('ACA_CareerServices')</v>
+        <v>mod_Accordion_ui('Aca_International Student and Scholar Services')</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -558,7 +585,7 @@
       </c>
       <c r="B5" s="3" t="str">
         <f>"mod_Accordion_server("&amp;"'"&amp;A2&amp;"', selector=selection, data="&amp;C2&amp;", title = c('"&amp;D2&amp;"'), Visible = T)"</f>
-        <v>mod_Accordion_server('ACA_CareerServices', selector=selection, data=ACAdata(), title = c('UAlbany Career Services'), Visible = T)</v>
+        <v>mod_Accordion_server('Aca_International Student and Scholar Services', selector=selection, data=Acadata(), title = c('International Student and Scholar Services'), Visible = T)</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -567,23 +594,26 @@
       </c>
       <c r="B6" s="3" t="str">
         <f>"mod_info_server('"&amp;A2&amp;"', selector = selection, data = "&amp;C2&amp;", rownametitle = c('"&amp;B2&amp;"'), phone = "&amp;E2&amp;", website = "&amp;F2&amp;")"</f>
-        <v>mod_info_server('ACA_CareerServices', selector = selection, data = ACAdata(), rownametitle = c('UAlbany Career Services'), phone = T, website = T)</v>
+        <v>mod_info_server('Aca_International Student and Scholar Services', selector = selection, data = Acadata(), rownametitle = c('International Student and Scholar Services'), phone = T, website = T)</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="C9" s="10"/>
       <c r="I9" s="11"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G10" s="1"/>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="5"/>
@@ -593,15 +623,15 @@
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A12" s="1"/>
       <c r="D12" s="5"/>
       <c r="E12" s="7"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B13" s="1"/>
       <c r="C13" s="8"/>
       <c r="D13" s="1"/>
@@ -612,10 +642,16 @@
       <c r="I13" s="9"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="C14" s="1"/>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="C15" s="1"/>
       <c r="E15" s="1"/>
     </row>
@@ -623,11 +659,38 @@
       <c r="C16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C18" s="4"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C20" s="4"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added NYS Smokers Quitline
</commit_message>
<xml_diff>
--- a/Module Code Generator.xlsx
+++ b/Module Code Generator.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intra\Desktop\Rolodex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intra\OneDrive\Desktop\Rolodex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21EEC3E-3AC1-4B89-A21E-7CAEE134B460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7E77C2-DBD1-479F-962A-96465F730128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{A9122E04-BE42-49C0-8E95-A2ED7E8620F5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Accordion Title</t>
   </si>
@@ -68,22 +68,34 @@
     <t>ENTER INTO UI</t>
   </si>
   <si>
-    <t>University Police (UPD)</t>
-  </si>
-  <si>
-    <t>Legaldata()</t>
-  </si>
-  <si>
-    <t>Legal_UPD</t>
-  </si>
-  <si>
-    <t>mod_Accordion_ui('Legal_UPD')</t>
-  </si>
-  <si>
-    <t>mod_Accordion_server('Legal_UPD', selector=selection, data=Legaldata(), title = c('University Police (UPD)'), Visible = T)</t>
-  </si>
-  <si>
-    <t>mod_info_server('Legal_UPD', selector = selection, data = Legaldata(), rownametitle = c('University Police (UPD)'), phone = T, website = T)</t>
+    <t>NY Quits - Smokers Quit Line</t>
+  </si>
+  <si>
+    <t>NYS Smokers Quit Line</t>
+  </si>
+  <si>
+    <t>mod_Accordion_ui('Hotline_NYSQuitline')</t>
+  </si>
+  <si>
+    <t>mod_Accordion_server('Hotline_NYSQuitline', selector=selection, data=HLdata(), title = c('NYS Smokers Quit Line'), Visible = T)</t>
+  </si>
+  <si>
+    <t>mod_info_server('Hotline_NYSQuitline', selector = selection, data = HLdata(), rownametitle = c('NY Quits - Smokers Quit Line'), phone = T, website = T)</t>
+  </si>
+  <si>
+    <t>AODdata()</t>
+  </si>
+  <si>
+    <t>AOD_NYSQuitline</t>
+  </si>
+  <si>
+    <t>mod_Accordion_ui('AOD_NYSQuitline')</t>
+  </si>
+  <si>
+    <t>mod_Accordion_server('AOD_NYSQuitline', selector=selection, data=AODdata(), title = c('NYS Smokers Quit Line'), Visible = T)</t>
+  </si>
+  <si>
+    <t>mod_info_server('AOD_NYSQuitline', selector = selection, data = AODdata(), rownametitle = c('NY Quits - Smokers Quit Line'), phone = T, website = T)</t>
   </si>
 </sst>
 </file>
@@ -498,7 +510,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A11"/>
+      <selection activeCell="A14" sqref="A14:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -534,16 +546,16 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>10</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>3</v>
@@ -558,7 +570,7 @@
       </c>
       <c r="B4" s="3" t="str">
         <f>"mod_Accordion_ui("&amp;"'"&amp;A2&amp;"'"&amp;")"</f>
-        <v>mod_Accordion_ui('Legal_UPD')</v>
+        <v>mod_Accordion_ui('AOD_NYSQuitline')</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -567,7 +579,7 @@
       </c>
       <c r="B5" s="3" t="str">
         <f>"mod_Accordion_server("&amp;"'"&amp;A2&amp;"', selector=selection, data="&amp;C2&amp;", title = c('"&amp;D2&amp;"'), Visible = T)"</f>
-        <v>mod_Accordion_server('Legal_UPD', selector=selection, data=Legaldata(), title = c('University Police (UPD)'), Visible = T)</v>
+        <v>mod_Accordion_server('AOD_NYSQuitline', selector=selection, data=AODdata(), title = c('NYS Smokers Quit Line'), Visible = T)</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -576,7 +588,7 @@
       </c>
       <c r="B6" s="3" t="str">
         <f>"mod_info_server('"&amp;A2&amp;"', selector = selection, data = "&amp;C2&amp;", rownametitle = c('"&amp;B2&amp;"'), phone = "&amp;E2&amp;", website = "&amp;F2&amp;")"</f>
-        <v>mod_info_server('Legal_UPD', selector = selection, data = Legaldata(), rownametitle = c('University Police (UPD)'), phone = T, website = T)</v>
+        <v>mod_info_server('AOD_NYSQuitline', selector = selection, data = AODdata(), rownametitle = c('NY Quits - Smokers Quit Line'), phone = T, website = T)</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -585,14 +597,14 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G9" s="1"/>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="5"/>
@@ -603,7 +615,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="7"/>
@@ -625,14 +637,23 @@
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="C14" s="1"/>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="C15" s="1"/>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="C16" s="1"/>
       <c r="E16" s="1"/>
     </row>

</xml_diff>

<commit_message>
Updates to PMH and FHF Resources
</commit_message>
<xml_diff>
--- a/Module Code Generator.xlsx
+++ b/Module Code Generator.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intra\OneDrive\Desktop\Rolodex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intra\OneDrive\Desktop\New Shiny Apps\Rolodex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7E77C2-DBD1-479F-962A-96465F730128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56BF014-41F5-4A8F-9155-B85D849AE67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{A9122E04-BE42-49C0-8E95-A2ED7E8620F5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Accordion Title</t>
   </si>
@@ -68,34 +68,40 @@
     <t>ENTER INTO UI</t>
   </si>
   <si>
-    <t>NY Quits - Smokers Quit Line</t>
-  </si>
-  <si>
-    <t>NYS Smokers Quit Line</t>
-  </si>
-  <si>
-    <t>mod_Accordion_ui('Hotline_NYSQuitline')</t>
-  </si>
-  <si>
-    <t>mod_Accordion_server('Hotline_NYSQuitline', selector=selection, data=HLdata(), title = c('NYS Smokers Quit Line'), Visible = T)</t>
-  </si>
-  <si>
-    <t>mod_info_server('Hotline_NYSQuitline', selector = selection, data = HLdata(), rownametitle = c('NY Quits - Smokers Quit Line'), phone = T, website = T)</t>
-  </si>
-  <si>
-    <t>AODdata()</t>
-  </si>
-  <si>
-    <t>AOD_NYSQuitline</t>
-  </si>
-  <si>
-    <t>mod_Accordion_ui('AOD_NYSQuitline')</t>
-  </si>
-  <si>
-    <t>mod_Accordion_server('AOD_NYSQuitline', selector=selection, data=AODdata(), title = c('NYS Smokers Quit Line'), Visible = T)</t>
-  </si>
-  <si>
-    <t>mod_info_server('AOD_NYSQuitline', selector = selection, data = AODdata(), rownametitle = c('NY Quits - Smokers Quit Line'), phone = T, website = T)</t>
+    <t>Off</t>
+  </si>
+  <si>
+    <t>FHF</t>
+  </si>
+  <si>
+    <t>Women’s Employment &amp; Resource Center (WERC)</t>
+  </si>
+  <si>
+    <t>155 Washington Avenue, 3rd Floor, Albany, NY 12210</t>
+  </si>
+  <si>
+    <t>tel:518-242-8249</t>
+  </si>
+  <si>
+    <t>https://www.cdwerc.org/student-services/Scholarships-96-pg.htm</t>
+  </si>
+  <si>
+    <t>WERC is a not-for-profit organization that works to advance women's success in the workplace by building their economic and personal independence.</t>
+  </si>
+  <si>
+    <t>FHFdata()</t>
+  </si>
+  <si>
+    <t>FHF_WERC</t>
+  </si>
+  <si>
+    <t>mod_Accordion_ui('FHF_WERC')</t>
+  </si>
+  <si>
+    <t>mod_Accordion_server('FHF_WERC', selector=selection, data=FHFdata(), title = c('Women’s Employment &amp; Resource Center (WERC)'), Visible = T)</t>
+  </si>
+  <si>
+    <t>mod_info_server('FHF_WERC', selector = selection, data = FHFdata(), rownametitle = c('Women’s Employment &amp; Resource Center (WERC)'), phone = T, website = T)</t>
   </si>
 </sst>
 </file>
@@ -132,13 +138,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -148,6 +147,13 @@
       <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -171,26 +177,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -507,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EBEBDEC-DB4C-4547-B739-F553404489A4}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:A16"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -546,16 +549,16 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>3</v>
@@ -570,7 +573,7 @@
       </c>
       <c r="B4" s="3" t="str">
         <f>"mod_Accordion_ui("&amp;"'"&amp;A2&amp;"'"&amp;")"</f>
-        <v>mod_Accordion_ui('AOD_NYSQuitline')</v>
+        <v>mod_Accordion_ui('FHF_WERC')</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -579,7 +582,7 @@
       </c>
       <c r="B5" s="3" t="str">
         <f>"mod_Accordion_server("&amp;"'"&amp;A2&amp;"', selector=selection, data="&amp;C2&amp;", title = c('"&amp;D2&amp;"'), Visible = T)"</f>
-        <v>mod_Accordion_server('AOD_NYSQuitline', selector=selection, data=AODdata(), title = c('NYS Smokers Quit Line'), Visible = T)</v>
+        <v>mod_Accordion_server('FHF_WERC', selector=selection, data=FHFdata(), title = c('Women’s Employment &amp; Resource Center (WERC)'), Visible = T)</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -588,97 +591,77 @@
       </c>
       <c r="B6" s="3" t="str">
         <f>"mod_info_server('"&amp;A2&amp;"', selector = selection, data = "&amp;C2&amp;", rownametitle = c('"&amp;B2&amp;"'), phone = "&amp;E2&amp;", website = "&amp;F2&amp;")"</f>
-        <v>mod_info_server('AOD_NYSQuitline', selector = selection, data = AODdata(), rownametitle = c('NY Quits - Smokers Quit Line'), phone = T, website = T)</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C8" s="10"/>
-      <c r="I8" s="11"/>
+        <v>mod_info_server('FHF_WERC', selector = selection, data = FHFdata(), rownametitle = c('Women’s Employment &amp; Resource Center (WERC)'), phone = T, website = T)</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+      <c r="B12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+      <c r="C12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="7"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="9"/>
+      <c r="D12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12"/>
+      <c r="G12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C13" s="1"/>
-      <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="C14" s="1"/>
-      <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="C15" s="4"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="12"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="7"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D12" r:id="rId1" xr:uid="{1461AAE1-ECC0-4E0F-A7D9-236641974F97}"/>
+    <hyperlink ref="C12" r:id="rId2" xr:uid="{12C569FE-7E23-4CCD-B13B-9BB253F1E074}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CHAMP Program Updated in AOD, MH, MHBC, MHLC, and Hotlines
</commit_message>
<xml_diff>
--- a/Module Code Generator.xlsx
+++ b/Module Code Generator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intra\OneDrive\Desktop\New Shiny Apps\Rolodex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56BF014-41F5-4A8F-9155-B85D849AE67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FADAD3-1CD5-4C4F-A6BA-F51097BED4B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{A9122E04-BE42-49C0-8E95-A2ED7E8620F5}"/>
+    <workbookView xWindow="6400" yWindow="0" windowWidth="19200" windowHeight="9970" xr2:uid="{A9122E04-BE42-49C0-8E95-A2ED7E8620F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Accordion Title</t>
   </si>
@@ -74,34 +74,34 @@
     <t>FHF</t>
   </si>
   <si>
-    <t>Women’s Employment &amp; Resource Center (WERC)</t>
-  </si>
-  <si>
-    <t>155 Washington Avenue, 3rd Floor, Albany, NY 12210</t>
-  </si>
-  <si>
-    <t>tel:518-242-8249</t>
-  </si>
-  <si>
-    <t>https://www.cdwerc.org/student-services/Scholarships-96-pg.htm</t>
-  </si>
-  <si>
     <t>WERC is a not-for-profit organization that works to advance women's success in the workplace by building their economic and personal independence.</t>
   </si>
   <si>
-    <t>FHFdata()</t>
-  </si>
-  <si>
-    <t>FHF_WERC</t>
-  </si>
-  <si>
-    <t>mod_Accordion_ui('FHF_WERC')</t>
-  </si>
-  <si>
-    <t>mod_Accordion_server('FHF_WERC', selector=selection, data=FHFdata(), title = c('Women’s Employment &amp; Resource Center (WERC)'), Visible = T)</t>
-  </si>
-  <si>
-    <t>mod_info_server('FHF_WERC', selector = selection, data = FHFdata(), rownametitle = c('Women’s Employment &amp; Resource Center (WERC)'), phone = T, website = T)</t>
+    <t>CHAMP Program (OASAS)</t>
+  </si>
+  <si>
+    <t>MHLC()</t>
+  </si>
+  <si>
+    <t>mod_Accordion_ui('MHBC_CHAMP')</t>
+  </si>
+  <si>
+    <t>mod_Accordion_server('MHBC_CHAMP', selector=selection, data=MHBC(), title = c('CHAMP Program (OASAS)'), Visible = T)</t>
+  </si>
+  <si>
+    <t>mod_info_server('MHBC_CHAMP', selector = selection, data = MHBC(), rownametitle = c('CHAMP Program (OASAS)'), phone = T, website = T)</t>
+  </si>
+  <si>
+    <t>MHLC_CHAMP</t>
+  </si>
+  <si>
+    <t>mod_Accordion_ui('MHLC_CHAMP')</t>
+  </si>
+  <si>
+    <t>mod_Accordion_server('MHLC_CHAMP', selector=selection, data=MHLC(), title = c('CHAMP Program (OASAS)'), Visible = T)</t>
+  </si>
+  <si>
+    <t>mod_info_server('MHLC_CHAMP', selector = selection, data = MHLC(), rownametitle = c('CHAMP Program (OASAS)'), phone = T, website = T)</t>
   </si>
 </sst>
 </file>
@@ -512,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EBEBDEC-DB4C-4547-B739-F553404489A4}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -551,14 +551,14 @@
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>3</v>
@@ -573,7 +573,7 @@
       </c>
       <c r="B4" s="3" t="str">
         <f>"mod_Accordion_ui("&amp;"'"&amp;A2&amp;"'"&amp;")"</f>
-        <v>mod_Accordion_ui('FHF_WERC')</v>
+        <v>mod_Accordion_ui('MHLC_CHAMP')</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -582,7 +582,7 @@
       </c>
       <c r="B5" s="3" t="str">
         <f>"mod_Accordion_server("&amp;"'"&amp;A2&amp;"', selector=selection, data="&amp;C2&amp;", title = c('"&amp;D2&amp;"'), Visible = T)"</f>
-        <v>mod_Accordion_server('FHF_WERC', selector=selection, data=FHFdata(), title = c('Women’s Employment &amp; Resource Center (WERC)'), Visible = T)</v>
+        <v>mod_Accordion_server('MHLC_CHAMP', selector=selection, data=MHLC(), title = c('CHAMP Program (OASAS)'), Visible = T)</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -591,39 +591,29 @@
       </c>
       <c r="B6" s="3" t="str">
         <f>"mod_info_server('"&amp;A2&amp;"', selector = selection, data = "&amp;C2&amp;", rownametitle = c('"&amp;B2&amp;"'), phone = "&amp;E2&amp;", website = "&amp;F2&amp;")"</f>
-        <v>mod_info_server('FHF_WERC', selector = selection, data = FHFdata(), rownametitle = c('Women’s Employment &amp; Resource Center (WERC)'), phone = T, website = T)</v>
+        <v>mod_info_server('MHLC_CHAMP', selector = selection, data = MHLC(), rownametitle = c('CHAMP Program (OASAS)'), phone = T, website = T)</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C11" s="5"/>
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>15</v>
-      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="10"/>
       <c r="E12" s="9"/>
       <c r="F12"/>
       <c r="G12" s="1" t="s">
@@ -633,16 +623,25 @@
         <v>10</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="C15" s="4"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -657,11 +656,7 @@
       <c r="I16" s="7"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D12" r:id="rId1" xr:uid="{1461AAE1-ECC0-4E0F-A7D9-236641974F97}"/>
-    <hyperlink ref="C12" r:id="rId2" xr:uid="{12C569FE-7E23-4CCD-B13B-9BB253F1E074}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added CURCE (Undergrad Research Center)
</commit_message>
<xml_diff>
--- a/Module Code Generator.xlsx
+++ b/Module Code Generator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intra\OneDrive\Desktop\New Shiny Apps\Rolodex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66543A68-1F88-4796-9E29-0ABBD8EACC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771C9D46-F900-4FDF-B624-67B2E0286A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="13770" xr2:uid="{A9122E04-BE42-49C0-8E95-A2ED7E8620F5}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="19200" windowHeight="9970" xr2:uid="{A9122E04-BE42-49C0-8E95-A2ED7E8620F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Accordion Title</t>
   </si>
@@ -68,29 +68,32 @@
     <t>ENTER INTO UI</t>
   </si>
   <si>
-    <t>AOD_St. Peter's Addiction Recovery</t>
-  </si>
-  <si>
-    <t>St. Peter's Addiction Recovery</t>
-  </si>
-  <si>
-    <t>AODdata()</t>
-  </si>
-  <si>
-    <t>mod_Accordion_ui('AOD_St. Peter's Addiction Recovery')</t>
-  </si>
-  <si>
-    <t>mod_Accordion_server('AOD_St. Peter's Addiction Recovery', selector=selection, data=AODdata(), title = c('St. Peter's Addiction Recovery'), Visible = T)</t>
-  </si>
-  <si>
-    <t>mod_info_server('AOD_St. Peter's Addiction Recovery', selector = selection, data = AODdata(), rownametitle = c('St. Peter's Addiction Recovery'), phone = T, website = T)</t>
+    <t>Center for Undergraduate Research and Creative Engagement (CURCE)</t>
+  </si>
+  <si>
+    <t>Aca_CURCE</t>
+  </si>
+  <si>
+    <t>Acadata()</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>mod_Accordion_ui('Aca_CURCE')</t>
+  </si>
+  <si>
+    <t>mod_Accordion_server('Aca_CURCE', selector=selection, data=Acadata(), title = c('Center for Undergraduate Research and Creative Engagement (CURCE)'), Visible = T)</t>
+  </si>
+  <si>
+    <t>mod_info_server('Aca_CURCE', selector = selection, data = Acadata(), rownametitle = c('Center for Undergraduate Research and Creative Engagement (CURCE)'), phone = F, website = T)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,12 +140,6 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF46166B"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -165,7 +162,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -182,9 +179,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -504,7 +498,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -540,19 +534,19 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>11</v>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>3</v>
@@ -564,7 +558,7 @@
       </c>
       <c r="B4" s="3" t="str">
         <f>"mod_Accordion_ui("&amp;"'"&amp;A2&amp;"'"&amp;")"</f>
-        <v>mod_Accordion_ui('AOD_St. Peter's Addiction Recovery')</v>
+        <v>mod_Accordion_ui('Aca_CURCE')</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -573,7 +567,7 @@
       </c>
       <c r="B5" s="3" t="str">
         <f>"mod_Accordion_server("&amp;"'"&amp;A2&amp;"', selector=selection, data="&amp;C2&amp;", title = c('"&amp;D2&amp;"'), Visible = T)"</f>
-        <v>mod_Accordion_server('AOD_St. Peter's Addiction Recovery', selector=selection, data=AODdata(), title = c('St. Peter's Addiction Recovery'), Visible = T)</v>
+        <v>mod_Accordion_server('Aca_CURCE', selector=selection, data=Acadata(), title = c('Center for Undergraduate Research and Creative Engagement (CURCE)'), Visible = T)</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -582,7 +576,22 @@
       </c>
       <c r="B6" s="3" t="str">
         <f>"mod_info_server('"&amp;A2&amp;"', selector = selection, data = "&amp;C2&amp;", rownametitle = c('"&amp;B2&amp;"'), phone = "&amp;E2&amp;", website = "&amp;F2&amp;")"</f>
-        <v>mod_info_server('AOD_St. Peter's Addiction Recovery', selector = selection, data = AODdata(), rownametitle = c('St. Peter's Addiction Recovery'), phone = T, website = T)</v>
+        <v>mod_info_server('Aca_CURCE', selector = selection, data = Acadata(), rownametitle = c('Center for Undergraduate Research and Creative Engagement (CURCE)'), phone = F, website = T)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -590,9 +599,6 @@
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="C12" s="5"/>
       <c r="D12" s="10"/>
       <c r="E12" s="9"/>
@@ -601,15 +607,9 @@
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
ICA included under Academic
</commit_message>
<xml_diff>
--- a/Module Code Generator.xlsx
+++ b/Module Code Generator.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intra\OneDrive\Desktop\New Shiny Apps\Rolodex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intra\Desktop\New Shiny Apps\Rolodex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771C9D46-F900-4FDF-B624-67B2E0286A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DD63FD-3C6A-4FC9-B34E-045D1476761A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="19200" windowHeight="9970" xr2:uid="{A9122E04-BE42-49C0-8E95-A2ED7E8620F5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{A9122E04-BE42-49C0-8E95-A2ED7E8620F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,25 +68,25 @@
     <t>ENTER INTO UI</t>
   </si>
   <si>
-    <t>Center for Undergraduate Research and Creative Engagement (CURCE)</t>
-  </si>
-  <si>
-    <t>Aca_CURCE</t>
-  </si>
-  <si>
     <t>Acadata()</t>
   </si>
   <si>
     <t>F</t>
   </si>
   <si>
-    <t>mod_Accordion_ui('Aca_CURCE')</t>
-  </si>
-  <si>
-    <t>mod_Accordion_server('Aca_CURCE', selector=selection, data=Acadata(), title = c('Center for Undergraduate Research and Creative Engagement (CURCE)'), Visible = T)</t>
-  </si>
-  <si>
-    <t>mod_info_server('Aca_CURCE', selector = selection, data = Acadata(), rownametitle = c('Center for Undergraduate Research and Creative Engagement (CURCE)'), phone = F, website = T)</t>
+    <t>International Crossroads Albany (ICA)</t>
+  </si>
+  <si>
+    <t>Aca_ICA</t>
+  </si>
+  <si>
+    <t>mod_Accordion_ui('Aca_ICA')</t>
+  </si>
+  <si>
+    <t>mod_Accordion_server('Aca_ICA', selector=selection, data=Acadata(), title = c('International Crossroads Albany (ICA)'), Visible = T)</t>
+  </si>
+  <si>
+    <t>mod_info_server('Aca_ICA', selector = selection, data = Acadata(), rownametitle = c('International Crossroads Albany (ICA)'), phone = F, website = T)</t>
   </si>
 </sst>
 </file>
@@ -498,7 +498,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A8" sqref="A8:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -534,19 +534,19 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>3</v>
@@ -558,7 +558,7 @@
       </c>
       <c r="B4" s="3" t="str">
         <f>"mod_Accordion_ui("&amp;"'"&amp;A2&amp;"'"&amp;")"</f>
-        <v>mod_Accordion_ui('Aca_CURCE')</v>
+        <v>mod_Accordion_ui('Aca_ICA')</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -567,7 +567,7 @@
       </c>
       <c r="B5" s="3" t="str">
         <f>"mod_Accordion_server("&amp;"'"&amp;A2&amp;"', selector=selection, data="&amp;C2&amp;", title = c('"&amp;D2&amp;"'), Visible = T)"</f>
-        <v>mod_Accordion_server('Aca_CURCE', selector=selection, data=Acadata(), title = c('Center for Undergraduate Research and Creative Engagement (CURCE)'), Visible = T)</v>
+        <v>mod_Accordion_server('Aca_ICA', selector=selection, data=Acadata(), title = c('International Crossroads Albany (ICA)'), Visible = T)</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -576,7 +576,7 @@
       </c>
       <c r="B6" s="3" t="str">
         <f>"mod_info_server('"&amp;A2&amp;"', selector = selection, data = "&amp;C2&amp;", rownametitle = c('"&amp;B2&amp;"'), phone = "&amp;E2&amp;", website = "&amp;F2&amp;")"</f>
-        <v>mod_info_server('Aca_CURCE', selector = selection, data = Acadata(), rownametitle = c('Center for Undergraduate Research and Creative Engagement (CURCE)'), phone = F, website = T)</v>
+        <v>mod_info_server('Aca_ICA', selector = selection, data = Acadata(), rownametitle = c('International Crossroads Albany (ICA)'), phone = F, website = T)</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added ISSS to International Accordion
</commit_message>
<xml_diff>
--- a/Module Code Generator.xlsx
+++ b/Module Code Generator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intra\Desktop\New Shiny Apps\Rolodex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7EE054-8120-4459-AD1F-9170D26F2EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF19EF6E-E724-45B4-87F2-3DDA269CCB2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{A9122E04-BE42-49C0-8E95-A2ED7E8620F5}"/>
   </bookViews>
@@ -71,50 +71,50 @@
     <t>On</t>
   </si>
   <si>
-    <t>Aca</t>
-  </si>
-  <si>
-    <t>Acadata()</t>
-  </si>
-  <si>
-    <t>University Interfaith Center</t>
-  </si>
-  <si>
-    <t>tel:5184425565</t>
-  </si>
-  <si>
-    <t>https://www.albany.edu/intercultural-student-engagement/interfaith-center</t>
-  </si>
-  <si>
-    <t>various times</t>
-  </si>
-  <si>
-    <t>ise@albany.edu</t>
-  </si>
-  <si>
-    <t>The Interfaith Center (IFC) has five chaplains and offers vibrant opportunities for spiritual practice, reflection, education and community building. We support faith and interfaith student groups by hosting dynamic events, inspiring religious services and serene spaces for meditation.</t>
-  </si>
-  <si>
-    <t>1400 Washington Avenue, Albany, NY 12222</t>
-  </si>
-  <si>
-    <t>Aca_InterfaithCenter</t>
-  </si>
-  <si>
-    <t>mod_Accordion_ui('Aca_InterfaithCenter')</t>
-  </si>
-  <si>
-    <t>mod_Accordion_server('Aca_InterfaithCenter', selector=selection, data=Acadata(), title = c('University Interfaith Center'), Visible = T)</t>
-  </si>
-  <si>
-    <t>mod_info_server('Aca_InterfaithCenter', selector = selection, data = Acadata(), rownametitle = c('University Interfaith Center'), phone = T, website = T)</t>
+    <t>International Student and Scholar Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Science Library G-40  </t>
+  </si>
+  <si>
+    <t>tel:(518)5918172</t>
+  </si>
+  <si>
+    <t>https://www.albany.edu/isss/</t>
+  </si>
+  <si>
+    <t>M, Tues, Th, F: 1 PM - 3:30 PM</t>
+  </si>
+  <si>
+    <t>ISSS@albany.edu</t>
+  </si>
+  <si>
+    <t>INTNL</t>
+  </si>
+  <si>
+    <t>Advising - workshops</t>
+  </si>
+  <si>
+    <t>INTNL_ISSS</t>
+  </si>
+  <si>
+    <t>INTNLdata()</t>
+  </si>
+  <si>
+    <t>mod_Accordion_ui('INTNL_ISSS')</t>
+  </si>
+  <si>
+    <t>mod_Accordion_server('INTNL_ISSS', selector=selection, data=INTNLdata(), title = c('International Student and Scholar Services'), Visible = T)</t>
+  </si>
+  <si>
+    <t>mod_info_server('INTNL_ISSS', selector = selection, data = INTNLdata(), rownametitle = c('International Student and Scholar Services'), phone = T, website = T)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,6 +156,11 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -178,24 +183,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -514,7 +516,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A13" sqref="A13:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -529,37 +531,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>13</v>
+      <c r="D2" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>3</v>
@@ -569,98 +571,93 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="1" t="str">
         <f>"mod_Accordion_ui("&amp;"'"&amp;A2&amp;"'"&amp;")"</f>
-        <v>mod_Accordion_ui('Aca_InterfaithCenter')</v>
+        <v>mod_Accordion_ui('INTNL_ISSS')</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="str">
         <f>"mod_Accordion_server("&amp;"'"&amp;A2&amp;"', selector=selection, data="&amp;C2&amp;", title = c('"&amp;D2&amp;"'), Visible = T)"</f>
-        <v>mod_Accordion_server('Aca_InterfaithCenter', selector=selection, data=Acadata(), title = c('University Interfaith Center'), Visible = T)</v>
+        <v>mod_Accordion_server('INTNL_ISSS', selector=selection, data=INTNLdata(), title = c('International Student and Scholar Services'), Visible = T)</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="1" t="str">
         <f>"mod_info_server('"&amp;A2&amp;"', selector = selection, data = "&amp;C2&amp;", rownametitle = c('"&amp;B2&amp;"'), phone = "&amp;E2&amp;", website = "&amp;F2&amp;")"</f>
-        <v>mod_info_server('Aca_InterfaithCenter', selector = selection, data = Acadata(), rownametitle = c('University Interfaith Center'), phone = T, website = T)</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
+        <v>mod_info_server('INTNL_ISSS', selector = selection, data = INTNLdata(), rownametitle = c('International Student and Scholar Services'), phone = T, website = T)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="E10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="F10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="G10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="I10" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C11" s="2"/>
-      <c r="I11" s="7"/>
+      <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C12" s="2"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="5"/>
-      <c r="I12" s="5"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="7"/>
+      <c r="F12"/>
+      <c r="G12" s="4"/>
+      <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="5"/>
+      <c r="C14" s="4"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="10"/>
+      <c r="C15" s="8"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F10" r:id="rId1" xr:uid="{7C679305-F587-4961-B756-81CAEF4C8126}"/>
-    <hyperlink ref="D10" r:id="rId2" xr:uid="{54496644-8E89-47F6-BBCB-31BED743F206}"/>
-    <hyperlink ref="C10" r:id="rId3" xr:uid="{01D57500-A413-4872-A13E-B7DBCF62B1DB}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added ICA to INTNL
</commit_message>
<xml_diff>
--- a/Module Code Generator.xlsx
+++ b/Module Code Generator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intra\Desktop\New Shiny Apps\Rolodex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF19EF6E-E724-45B4-87F2-3DDA269CCB2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5253B137-5156-43D2-97F4-7270368B7BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{A9122E04-BE42-49C0-8E95-A2ED7E8620F5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Accordion Title</t>
   </si>
@@ -68,36 +68,9 @@
     <t>ENTER INTO UI</t>
   </si>
   <si>
-    <t>On</t>
-  </si>
-  <si>
-    <t>International Student and Scholar Services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Science Library G-40  </t>
-  </si>
-  <si>
-    <t>tel:(518)5918172</t>
-  </si>
-  <si>
-    <t>https://www.albany.edu/isss/</t>
-  </si>
-  <si>
-    <t>M, Tues, Th, F: 1 PM - 3:30 PM</t>
-  </si>
-  <si>
-    <t>ISSS@albany.edu</t>
-  </si>
-  <si>
     <t>INTNL</t>
   </si>
   <si>
-    <t>Advising - workshops</t>
-  </si>
-  <si>
-    <t>INTNL_ISSS</t>
-  </si>
-  <si>
     <t>INTNLdata()</t>
   </si>
   <si>
@@ -108,13 +81,37 @@
   </si>
   <si>
     <t>mod_info_server('INTNL_ISSS', selector = selection, data = INTNLdata(), rownametitle = c('International Student and Scholar Services'), phone = T, website = T)</t>
+  </si>
+  <si>
+    <t>International Crossroads Albany (ICA)</t>
+  </si>
+  <si>
+    <t>tel:(518)396-6025</t>
+  </si>
+  <si>
+    <t>https://www.icalbany.org/</t>
+  </si>
+  <si>
+    <t>mark@internationalcrossroads.org</t>
+  </si>
+  <si>
+    <t>Off</t>
+  </si>
+  <si>
+    <t>ICA offers events and community for international students - primarily serves internationals at RPI, U Albany, and Union College - open to all internationals in the Capital District - activities enhance experience and understanding of American culture - includes large events, Friendship Partner Program, conversational English groups, and Bible discussions.</t>
+  </si>
+  <si>
+    <t>INTNL_ICA</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,11 +153,6 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -183,7 +175,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
@@ -197,7 +189,8 @@
       <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -513,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EBEBDEC-DB4C-4547-B739-F553404489A4}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:A15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -552,19 +545,19 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>11</v>
+      <c r="D2" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>3</v>
@@ -576,7 +569,7 @@
       </c>
       <c r="B4" s="1" t="str">
         <f>"mod_Accordion_ui("&amp;"'"&amp;A2&amp;"'"&amp;")"</f>
-        <v>mod_Accordion_ui('INTNL_ISSS')</v>
+        <v>mod_Accordion_ui('INTNL_ICA')</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -585,7 +578,7 @@
       </c>
       <c r="B5" s="1" t="str">
         <f>"mod_Accordion_server("&amp;"'"&amp;A2&amp;"', selector=selection, data="&amp;C2&amp;", title = c('"&amp;D2&amp;"'), Visible = T)"</f>
-        <v>mod_Accordion_server('INTNL_ISSS', selector=selection, data=INTNLdata(), title = c('International Student and Scholar Services'), Visible = T)</v>
+        <v>mod_Accordion_server('INTNL_ICA', selector=selection, data=INTNLdata(), title = c('International Crossroads Albany (ICA)'), Visible = T)</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -594,70 +587,68 @@
       </c>
       <c r="B6" s="1" t="str">
         <f>"mod_info_server('"&amp;A2&amp;"', selector = selection, data = "&amp;C2&amp;", rownametitle = c('"&amp;B2&amp;"'), phone = "&amp;E2&amp;", website = "&amp;F2&amp;")"</f>
-        <v>mod_info_server('INTNL_ISSS', selector = selection, data = INTNLdata(), rownametitle = c('International Student and Scholar Services'), phone = T, website = T)</v>
+        <v>mod_info_server('INTNL_ICA', selector = selection, data = INTNLdata(), rownametitle = c('International Crossroads Albany (ICA)'), phone = F, website = T)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>18</v>
-      </c>
+      <c r="C10" s="2"/>
+      <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C11" s="2"/>
-      <c r="I11" s="5"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="7"/>
+      <c r="F11"/>
+      <c r="G11" s="4"/>
+      <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C12" s="2"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
-      <c r="F12"/>
-      <c r="G12" s="4"/>
-      <c r="I12" s="4"/>
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="4"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="8"/>
+        <v>14</v>
+      </c>
+      <c r="C14" s="8"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C9" r:id="rId1" xr:uid="{3BCC2413-4D3D-442B-AFEC-278941669B7A}"/>
+    <hyperlink ref="D9" r:id="rId2" xr:uid="{8C3478BC-84BB-448F-A458-7C668DAD26C4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>